<commit_message>
Advection tests with smaller dt
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/advect_tests/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/advect_tests/mass_conserv_advect.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="480" windowWidth="16240" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="21540" yWindow="460" windowWidth="16240" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Case</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>New 200m avg vel, dt = 1 hr, j = 2, swim to deep, mult by lmask 1st</t>
+  </si>
+  <si>
+    <t>New 200m avg vel, dt = 1 hr, j = 2, swim to const rand, mult by lmask 1st</t>
+  </si>
+  <si>
+    <t>New 200m avg vel, dt = 1 hr, j = 2, swim to changing rand, mult by lmask 1st</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -205,7 +211,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,7 +494,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,6 +846,44 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
+    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7">
+        <v>2.6601999999999998E+37</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7">
+        <v>3.1471000000000002E+46</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7">
+        <v>1.5424999999999999E+42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6">
+        <v>4.7473000000000001</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
+        <v>161.745</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6">
+        <v>177.05170000000001</v>
+      </c>
+    </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>19</v>

</xml_diff>